<commit_message>
Carat: Fix reports issues
</commit_message>
<xml_diff>
--- a/Carat/templates/DefaultBySubject.xlsx
+++ b/Carat/templates/DefaultBySubject.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -131,35 +131,38 @@
     <t>з магістрами</t>
   </si>
   <si>
+    <t>бакалаврів</t>
+  </si>
+  <si>
+    <t>магістр ОПП</t>
+  </si>
+  <si>
+    <t>магістр ОНП</t>
+  </si>
+  <si>
+    <t>аспірантами</t>
+  </si>
+  <si>
+    <t>здобувач., стаж.</t>
+  </si>
+  <si>
+    <t>Всього по кафедрі:</t>
+  </si>
+  <si>
+    <t>ПІБ</t>
+  </si>
+  <si>
+    <t>Звіт за вибраною дисципліною</t>
+  </si>
+  <si>
+    <t>Групи</t>
+  </si>
+  <si>
     <t>за змішаною
-формою начвання</t>
-  </si>
-  <si>
-    <t>бакалаврів</t>
-  </si>
-  <si>
-    <t>магістр ОПП</t>
-  </si>
-  <si>
-    <t>магістр ОНП</t>
-  </si>
-  <si>
-    <t>аспірантами</t>
-  </si>
-  <si>
-    <t>здобувач., стаж.</t>
-  </si>
-  <si>
-    <t>Всього по кафедрі:</t>
-  </si>
-  <si>
-    <t>ПІБ</t>
-  </si>
-  <si>
-    <t>Звіт за вибраною дисципліною</t>
-  </si>
-  <si>
-    <t>Групи</t>
+формою навчання</t>
+  </si>
+  <si>
+    <t>аспірантів</t>
   </si>
 </sst>
 </file>
@@ -454,6 +457,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
     </xf>
@@ -466,11 +475,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -482,15 +494,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -773,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8:AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +813,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -910,63 +913,63 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:41" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="29" t="s">
+      <c r="O7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="30" t="s">
+      <c r="R7" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="31"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="33" t="s">
+      <c r="S7" s="33"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="29" t="s">
         <v>21</v>
       </c>
       <c r="V7" s="26" t="s">
@@ -1009,23 +1012,23 @@
       </c>
     </row>
     <row r="8" spans="1:41" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
       <c r="R8" s="8" t="s">
         <v>31</v>
       </c>
@@ -1033,35 +1036,35 @@
         <v>32</v>
       </c>
       <c r="T8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" s="30"/>
+      <c r="V8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="U8" s="34"/>
-      <c r="V8" s="8" t="s">
+      <c r="W8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="W8" s="8" t="s">
+      <c r="X8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="X8" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="Y8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="8" t="s">
+      <c r="AA8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AA8" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="AB8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AC8" s="8" t="s">
+      <c r="AD8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="AD8" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="AE8" s="8" t="s">
         <v>34</v>
@@ -1070,22 +1073,22 @@
         <v>35</v>
       </c>
       <c r="AG8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AH8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK8" s="10" t="s">
+      <c r="AL8" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="AL8" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="AM8" s="23"/>
       <c r="AN8" s="23"/>
@@ -1137,7 +1140,7 @@
     <row r="10" spans="1:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>

</xml_diff>

<commit_message>
Carat: Add EducForm in reports
</commit_message>
<xml_diff>
--- a/Carat/templates/DefaultBySubject.xlsx
+++ b/Carat/templates/DefaultBySubject.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>аспірантів</t>
+  </si>
+  <si>
+    <t>Форма навчання</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -494,6 +497,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -774,48 +783,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO10"/>
+  <dimension ref="A1:AP10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8:AG8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="1"/>
-      <c r="AC2" s="2" t="s">
+      <c r="AB2" s="1"/>
+      <c r="AD2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -836,10 +847,11 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="4"/>
-      <c r="AC3" s="6"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="4"/>
+      <c r="AD3" s="6"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -871,8 +883,9 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -905,14 +918,15 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:41" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>5</v>
       </c>
@@ -925,98 +939,101 @@
       <c r="D7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="G7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="H7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="I7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="J7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="K7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="L7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="M7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="N7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="O7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="31" t="s">
+      <c r="P7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="31" t="s">
+      <c r="Q7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="R7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="S7" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="33"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="29" t="s">
+      <c r="T7" s="33"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="V7" s="26" t="s">
+      <c r="W7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="W7" s="26"/>
       <c r="X7" s="26"/>
-      <c r="Y7" s="26" t="s">
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Z7" s="26"/>
       <c r="AA7" s="26"/>
-      <c r="AB7" s="27" t="s">
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AC7" s="27"/>
       <c r="AD7" s="27"/>
-      <c r="AE7" s="27" t="s">
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AF7" s="28"/>
       <c r="AG7" s="28"/>
-      <c r="AH7" s="26" t="s">
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AI7" s="26"/>
       <c r="AJ7" s="26"/>
-      <c r="AK7" s="26" t="s">
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AL7" s="26"/>
-      <c r="AM7" s="22" t="s">
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AN7" s="22" t="s">
+      <c r="AO7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AO7" s="24" t="s">
+      <c r="AP7" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="39"/>
       <c r="B8" s="41"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
-      <c r="E8" s="31"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
@@ -1029,78 +1046,79 @@
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="31"/>
+      <c r="S8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="T8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="U8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="30"/>
-      <c r="V8" s="8" t="s">
+      <c r="V8" s="30"/>
+      <c r="W8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="W8" s="8" t="s">
+      <c r="X8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="X8" s="8" t="s">
+      <c r="Y8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="8" t="s">
+      <c r="Z8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Z8" s="8" t="s">
+      <c r="AA8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AB8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AB8" s="8" t="s">
+      <c r="AC8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AC8" s="8" t="s">
+      <c r="AD8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AD8" s="8" t="s">
+      <c r="AE8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AE8" s="8" t="s">
+      <c r="AF8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AF8" s="8" t="s">
+      <c r="AG8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AG8" s="8" t="s">
+      <c r="AH8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AH8" s="8" t="s">
+      <c r="AI8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AI8" s="8" t="s">
+      <c r="AJ8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ8" s="8" t="s">
+      <c r="AK8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK8" s="10" t="s">
+      <c r="AL8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AL8" s="10" t="s">
+      <c r="AM8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AM8" s="23"/>
       <c r="AN8" s="23"/>
-      <c r="AO8" s="25"/>
+      <c r="AO8" s="23"/>
+      <c r="AP8" s="25"/>
     </row>
-    <row r="9" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -1135,26 +1153,24 @@
       <c r="AL9" s="15"/>
       <c r="AM9" s="15"/>
       <c r="AN9" s="15"/>
-      <c r="AO9" s="16"/>
+      <c r="AO9" s="15"/>
+      <c r="AP9" s="16"/>
     </row>
-    <row r="10" spans="1:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20">
-        <f>SUM(F9:F9)</f>
-        <v>0</v>
-      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="20">
-        <f t="shared" ref="G10:AN10" si="0">SUM(G9:G9)</f>
+        <f>SUM(G9:G9)</f>
         <v>0</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H10:AO10" si="0">SUM(H9:H9)</f>
         <v>0</v>
       </c>
       <c r="I10" s="20">
@@ -1197,11 +1213,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="20"/>
       <c r="U10" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1282,22 +1298,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AO10" s="21">
-        <f t="shared" ref="AO10" si="1">SUM(F10:AN10)</f>
+      <c r="AO10" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP10" s="21">
+        <f t="shared" ref="AP10" si="1">SUM(G10:AO10)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="G7:G8"/>
+  <mergeCells count="29">
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="V7:V8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
@@ -1307,16 +1327,17 @@
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="P7:P8"/>
     <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="AM7:AM8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:U7"/>
     <mergeCell ref="AN7:AN8"/>
     <mergeCell ref="AO7:AO8"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AH7:AJ7"/>
-    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AP7:AP8"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="AC7:AE7"/>
+    <mergeCell ref="AF7:AH7"/>
+    <mergeCell ref="AI7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>